<commit_message>
corrected ranks in correlation analysis
</commit_message>
<xml_diff>
--- a/Apache Commons Collection/Code churn/code churn.xlsx
+++ b/Apache Commons Collection/Code churn/code churn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subhannitasarcar/Documents/GitHub/SOEN6611/SOEN6611_TeamS/Apache Commons Collection/Code churn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAF0FCB-BF8D-5041-B453-4A0AD3FACCEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582E7E57-3031-194A-BD31-D0083A82C2E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="27500" windowHeight="17540" xr2:uid="{63FFF5D8-DB16-9046-B4A9-933F626992D1}"/>
+    <workbookView xWindow="3800" yWindow="1060" windowWidth="27500" windowHeight="17540" xr2:uid="{63FFF5D8-DB16-9046-B4A9-933F626992D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,28 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16632269-42FE-FC47-8ED3-5E51048CA9AE}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,9 +558,9 @@
         <f t="shared" ref="E3:E12" si="0">B3+C3+D3</f>
         <v>495</v>
       </c>
-      <c r="F3" t="e" cm="1">
-        <f t="array" ref="F3">F2+F18E3</f>
-        <v>#NAME?</v>
+      <c r="F3">
+        <f>F2+E3</f>
+        <v>978</v>
       </c>
       <c r="G3">
         <f>(E3+F2)/2</f>
@@ -606,13 +584,13 @@
         <f t="shared" si="0"/>
         <v>509</v>
       </c>
-      <c r="F4" t="e">
-        <f t="shared" ref="F4:F12" si="1">F3+E4</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G4" t="e">
+      <c r="F4">
+        <f>F3+E4</f>
+        <v>1487</v>
+      </c>
+      <c r="G4">
         <f>(E4+F3)/2</f>
-        <v>#NAME?</v>
+        <v>743.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -632,13 +610,13 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="F5" t="e">
-        <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G5" t="e">
+      <c r="F5">
+        <f t="shared" ref="F4:F12" si="1">F4+E5</f>
+        <v>1540</v>
+      </c>
+      <c r="G5">
         <f t="shared" ref="G5:G12" si="2">(E5+F4)/2</f>
-        <v>#NAME?</v>
+        <v>770</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -658,13 +636,13 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="F6" t="e">
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G6" t="e">
+        <v>2540</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -684,13 +662,13 @@
         <f t="shared" si="0"/>
         <v>306</v>
       </c>
-      <c r="F7" t="e">
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G7" t="e">
+        <v>2846</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -710,13 +688,13 @@
         <f t="shared" si="0"/>
         <v>301</v>
       </c>
-      <c r="F8" t="e">
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G8" t="e">
+        <v>3147</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>1573.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -736,13 +714,13 @@
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
-      <c r="F9" t="e">
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G9" t="e">
+        <v>3699</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>1849.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -762,13 +740,13 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F10" t="e">
+      <c r="F10">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G10" t="e">
+        <v>3723</v>
+      </c>
+      <c r="G10">
         <f>(E10+F9)/2</f>
-        <v>#NAME?</v>
+        <v>1861.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -788,13 +766,13 @@
         <f t="shared" si="0"/>
         <v>260</v>
       </c>
-      <c r="F11" t="e">
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G11" t="e">
+        <v>3983</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>1991.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,13 +792,13 @@
         <f t="shared" si="0"/>
         <v>430</v>
       </c>
-      <c r="F12" t="e">
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G12" t="e">
+        <v>4413</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="2"/>
-        <v>#NAME?</v>
+        <v>2206.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>